<commit_message>
updated the spread sheet and started the template for the report
</commit_message>
<xml_diff>
--- a/Financial Models.xlsx
+++ b/Financial Models.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Publisher Max Sales" sheetId="1" r:id="rId1"/>
@@ -495,9 +495,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J28" sqref="J28"/>
+      <selection pane="topRight" activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,13 +603,13 @@
         <v>75000</v>
       </c>
       <c r="Q5">
-        <v>75000</v>
+        <v>100000</v>
       </c>
       <c r="R5">
-        <v>75000</v>
+        <v>100000</v>
       </c>
       <c r="S5">
-        <v>75000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -678,15 +678,15 @@
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>75000</v>
+        <v>100000</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>75000</v>
+        <v>100000</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>75000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1040,13 +1040,10 @@
         <v>150000</v>
       </c>
       <c r="Q21">
-        <v>75000</v>
+        <v>100000</v>
       </c>
       <c r="R21">
-        <v>75000</v>
-      </c>
-      <c r="S21">
-        <v>50000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -1060,7 +1057,7 @@
         <v>37500</v>
       </c>
       <c r="S22">
-        <v>12500</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -1129,15 +1126,15 @@
       </c>
       <c r="Q24">
         <f t="shared" si="2"/>
-        <v>125000</v>
+        <v>150000</v>
       </c>
       <c r="R24">
         <f t="shared" si="2"/>
-        <v>125000</v>
+        <v>150000</v>
       </c>
       <c r="S24">
         <f t="shared" si="2"/>
-        <v>62500</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -1214,7 +1211,7 @@
       </c>
       <c r="S26">
         <f t="shared" si="4"/>
-        <v>12500</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -1291,7 +1288,7 @@
       </c>
       <c r="S28">
         <f t="shared" si="5"/>
-        <v>119000</v>
+        <v>156500</v>
       </c>
     </row>
   </sheetData>
@@ -1304,7 +1301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G5" sqref="G5"/>
     </sheetView>

</xml_diff>

<commit_message>
added some colouring to the spreadsheet
</commit_message>
<xml_diff>
--- a/Financial Models.xlsx
+++ b/Financial Models.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Publisher Max Sales" sheetId="1" r:id="rId1"/>
@@ -217,7 +217,68 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -495,9 +556,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T21" sqref="T21"/>
+      <selection pane="topRight" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,11 +1203,11 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:M26" si="3">B7-B24</f>
+        <f>B7-B24</f>
         <v>134800</v>
       </c>
       <c r="C26">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B26:M26" si="3">C7-C24</f>
         <v>-15200</v>
       </c>
       <c r="D26">
@@ -1292,6 +1353,14 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B26:S26">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1303,7 +1372,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G5" sqref="G5"/>
+      <selection pane="topRight" activeCell="B26" sqref="B26:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,6 +1889,14 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B26:J26">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1828,7 +1905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="L9" sqref="L9"/>
     </sheetView>

</xml_diff>

<commit_message>
I did work good
</commit_message>
<xml_diff>
--- a/Financial Models.xlsx
+++ b/Financial Models.xlsx
@@ -9,12 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Publisher Max Sales" sheetId="1" r:id="rId1"/>
     <sheet name="Publisher Min Sales" sheetId="2" r:id="rId2"/>
     <sheet name="Self-Publishing" sheetId="3" r:id="rId3"/>
+    <sheet name="Self-Publishing Sales" sheetId="4" r:id="rId4"/>
+    <sheet name="Publishing Sales" sheetId="5" r:id="rId5"/>
+    <sheet name="Self-Publishing Dev" sheetId="6" r:id="rId6"/>
+    <sheet name="Publishing Dev" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
   <si>
     <t>Revenues</t>
   </si>
@@ -152,6 +156,75 @@
   </si>
   <si>
     <t>Net Sales</t>
+  </si>
+  <si>
+    <t>Prototyping new IP?</t>
+  </si>
+  <si>
+    <t>Month 1</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Itch.io</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>NET</t>
+  </si>
+  <si>
+    <t>Rev.(£)</t>
+  </si>
+  <si>
+    <t>Total Income</t>
+  </si>
+  <si>
+    <t>Outgoing</t>
+  </si>
+  <si>
+    <t>Advertising</t>
+  </si>
+  <si>
+    <t>Total Outgoing</t>
+  </si>
+  <si>
+    <t>Monthly Profit</t>
+  </si>
+  <si>
+    <t>Profit B/F (£)</t>
+  </si>
+  <si>
+    <t>Month 2</t>
+  </si>
+  <si>
+    <t>Month 3</t>
+  </si>
+  <si>
+    <t>Month 4</t>
+  </si>
+  <si>
+    <t>Month 5</t>
+  </si>
+  <si>
+    <t>Month 6</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Beta Testing</t>
+  </si>
+  <si>
+    <t>Bug Fixing</t>
+  </si>
+  <si>
+    <t>Sign Off</t>
   </si>
 </sst>
 </file>
@@ -175,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,8 +267,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -203,21 +294,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -245,16 +419,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -538,7 +702,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N20" sqref="N20"/>
+      <selection pane="topRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,10 +1498,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B26:S26">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1350,7 +1514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="K17" sqref="K17"/>
     </sheetView>
@@ -1861,10 +2025,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B26:J26">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1874,11 +2038,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L9" sqref="L9"/>
+      <selection pane="topRight" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,6 +2079,12 @@
       <c r="J1" t="s">
         <v>11</v>
       </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1926,13 +2096,19 @@
         <v>16</v>
       </c>
       <c r="H3">
+        <v>5000</v>
+      </c>
+      <c r="I3">
+        <v>10000</v>
+      </c>
+      <c r="J3">
         <v>20000</v>
       </c>
-      <c r="I3">
-        <v>20000</v>
-      </c>
-      <c r="J3">
+      <c r="K3">
         <v>10000</v>
+      </c>
+      <c r="L3">
+        <v>5000</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1940,7 +2116,7 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:J5" si="0">SUM(B3:B3)</f>
+        <f t="shared" ref="B5:L5" si="0">SUM(B3:B3)</f>
         <v>0</v>
       </c>
       <c r="C5">
@@ -1965,15 +2141,23 @@
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>20000</v>
+        <v>5000</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
         <v>10000</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>5000</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1991,7 +2175,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -2024,17 +2208,25 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <f>H5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="I9">
-        <f t="shared" ref="I9:J9" si="1">I5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="J9">
+      <c r="H9" s="5">
+        <f>(H5-H17)/7</f>
+        <v>642.85714285714289</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" ref="I9:L9" si="1">(I5-I17)/7</f>
+        <v>1285.7142857142858</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="1"/>
+        <v>2571.4285714285716</v>
+      </c>
+      <c r="K9" s="5">
         <f t="shared" si="1"/>
         <v>1428.5714285714287</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" si="1"/>
+        <v>714.28571428571433</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2059,17 +2251,25 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <f>H5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="I10">
-        <f t="shared" ref="I10:J10" si="2">I5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="J10">
+      <c r="H10" s="5">
+        <f>(H5-H17)/7</f>
+        <v>642.85714285714289</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" ref="I10:L10" si="2">(I5-I17)/7</f>
+        <v>1285.7142857142858</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="2"/>
+        <v>2571.4285714285716</v>
+      </c>
+      <c r="K10" s="5">
         <f t="shared" si="2"/>
         <v>1428.5714285714287</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" si="2"/>
+        <v>714.28571428571433</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2094,17 +2294,25 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <f>H5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="I11">
-        <f t="shared" ref="I11:J11" si="3">I5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="J11">
+      <c r="H11" s="5">
+        <f>(H5-H17)/7</f>
+        <v>642.85714285714289</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" ref="I11:L11" si="3">(I5-I17)/7</f>
+        <v>1285.7142857142858</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="3"/>
+        <v>2571.4285714285716</v>
+      </c>
+      <c r="K11" s="5">
         <f t="shared" si="3"/>
         <v>1428.5714285714287</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" si="3"/>
+        <v>714.28571428571433</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2129,17 +2337,25 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12">
-        <f>H5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="I12">
-        <f t="shared" ref="I12:J12" si="4">I5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="J12">
+      <c r="H12" s="5">
+        <f>(H5-H17)/7</f>
+        <v>642.85714285714289</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" ref="I12:L12" si="4">(I5-I17)/7</f>
+        <v>1285.7142857142858</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="4"/>
+        <v>2571.4285714285716</v>
+      </c>
+      <c r="K12" s="5">
         <f t="shared" si="4"/>
         <v>1428.5714285714287</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="4"/>
+        <v>714.28571428571433</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2164,17 +2380,25 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <f>H5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="I13">
-        <f t="shared" ref="I13:J13" si="5">I5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="J13">
+      <c r="H13" s="5">
+        <f>(H5-H17)/7</f>
+        <v>642.85714285714289</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" ref="I13:L13" si="5">(I5-I17)/7</f>
+        <v>1285.7142857142858</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="5"/>
+        <v>2571.4285714285716</v>
+      </c>
+      <c r="K13" s="5">
         <f t="shared" si="5"/>
         <v>1428.5714285714287</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="5"/>
+        <v>714.28571428571433</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2199,17 +2423,25 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14">
-        <f>H5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="I14">
-        <f t="shared" ref="I14:J14" si="6">I5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="J14">
+      <c r="H14" s="5">
+        <f>(H5-H17)/7</f>
+        <v>642.85714285714289</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" ref="I14:L14" si="6">(I5-I17)/7</f>
+        <v>1285.7142857142858</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="6"/>
+        <v>2571.4285714285716</v>
+      </c>
+      <c r="K14" s="5">
         <f t="shared" si="6"/>
         <v>1428.5714285714287</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" si="6"/>
+        <v>714.28571428571433</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2234,143 +2466,964 @@
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="H15">
-        <f>H5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="I15">
-        <f t="shared" ref="I15:J15" si="7">I5/7</f>
-        <v>2857.1428571428573</v>
-      </c>
-      <c r="J15">
+      <c r="H15" s="5">
+        <f>(H5-H17)/7</f>
+        <v>642.85714285714289</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" ref="I15:L15" si="7">(I5-I17)/7</f>
+        <v>1285.7142857142858</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="7"/>
+        <v>2571.4285714285716</v>
+      </c>
+      <c r="K15" s="5">
         <f t="shared" si="7"/>
         <v>1428.5714285714287</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="L15" s="5">
+        <f t="shared" si="7"/>
+        <v>714.28571428571433</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17">
+        <f>H5*0.1</f>
+        <v>500</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:J17" si="8">I5*0.1</f>
+        <v>1000</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="8"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18">
-        <f t="shared" ref="B18:J18" si="8">SUM(B8:B16)</f>
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="8"/>
+      <c r="B19">
+        <f t="shared" ref="B19:J19" si="9">SUM(B8:B17)</f>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="9"/>
+        <v>5000.0000000000009</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="9"/>
+        <v>10000.000000000002</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="9"/>
         <v>20000.000000000004</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="8"/>
-        <v>20000.000000000004</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="8"/>
+      <c r="K19">
+        <f t="shared" ref="K19:L19" si="10">SUM(K8:K17)</f>
         <v>10000.000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="L19">
+        <f t="shared" si="10"/>
+        <v>5000.0000000000009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B20">
-        <f t="shared" ref="B20:J20" si="9">B5-B18</f>
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B21">
+        <f t="shared" ref="B21:J21" si="11">B5-B19</f>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21:L21" si="12">K5-K19</f>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B22">
-        <f>B20</f>
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <f>B22+C20</f>
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <f t="shared" ref="D22:J22" si="10">C22+D20</f>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="10"/>
+      <c r="B23">
+        <f>B21</f>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>B23+C21</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:J23" si="13">C23+D21</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ref="K23" si="14">J23+K21</f>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ref="L23" si="15">K23+L21</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>4000</v>
+      </c>
+      <c r="E4">
+        <v>2000</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="4">
+        <f>B5*B4</f>
+        <v>5000</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" ref="C6:F6" si="0">C5*C4</f>
+        <v>10000</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="7">
+        <f>B6</f>
+        <v>5000</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" ref="C8:F8" si="1">C6</f>
+        <v>10000</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11">
+        <f>B8*0.1</f>
+        <v>500</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="2">C8*0.1</f>
+        <v>1000</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="7">
+        <f>B11</f>
+        <v>500</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" ref="C13:F13" si="3">C11</f>
+        <v>1000</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="3"/>
+        <v>2000</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15">
+        <f>B8-B13</f>
+        <v>4500</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:F15" si="4">C8-C13</f>
+        <v>9000</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="4"/>
+        <v>18000</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="7">
+        <f>B15</f>
+        <v>4500</v>
+      </c>
+      <c r="C17" s="7">
+        <f>C15+B17</f>
+        <v>13500</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" ref="D17:F17" si="5">D15+C17</f>
+        <v>31500</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="5"/>
+        <v>41500</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="5"/>
+        <v>46500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="25" width="2.7109375" customWidth="1"/>
+    <col min="26" max="26" width="2.28515625" customWidth="1"/>
+    <col min="27" max="27" width="2.42578125" customWidth="1"/>
+    <col min="28" max="28" width="2.28515625" customWidth="1"/>
+    <col min="29" max="29" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="13"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9">
+        <v>3</v>
+      </c>
+      <c r="E2" s="9">
+        <v>4</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9">
+        <v>2</v>
+      </c>
+      <c r="H2" s="9">
+        <v>3</v>
+      </c>
+      <c r="I2" s="9">
+        <v>4</v>
+      </c>
+      <c r="J2" s="9">
+        <v>1</v>
+      </c>
+      <c r="K2" s="9">
+        <v>2</v>
+      </c>
+      <c r="L2" s="9">
+        <v>3</v>
+      </c>
+      <c r="M2" s="9">
+        <v>4</v>
+      </c>
+      <c r="N2" s="9">
+        <v>1</v>
+      </c>
+      <c r="O2" s="9">
+        <v>2</v>
+      </c>
+      <c r="P2" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>4</v>
+      </c>
+      <c r="R2" s="9">
+        <v>1</v>
+      </c>
+      <c r="S2" s="9">
+        <v>2</v>
+      </c>
+      <c r="T2" s="9">
+        <v>3</v>
+      </c>
+      <c r="U2" s="9">
+        <v>4</v>
+      </c>
+      <c r="V2" s="9">
+        <v>1</v>
+      </c>
+      <c r="W2" s="9">
+        <v>2</v>
+      </c>
+      <c r="X2" s="9">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="9">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="9">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
spread sheets done, marketing talked about
</commit_message>
<xml_diff>
--- a/Financial Models.xlsx
+++ b/Financial Models.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Publisher Max Sales" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="73">
   <si>
     <t>Revenues</t>
   </si>
@@ -225,6 +225,30 @@
   </si>
   <si>
     <t>Sign Off</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>Revenue Share</t>
+  </si>
+  <si>
+    <t>Playstation</t>
+  </si>
+  <si>
+    <t>Xbox</t>
+  </si>
+  <si>
+    <t>Inestment Repay</t>
+  </si>
+  <si>
+    <t>Investment Repay</t>
+  </si>
+  <si>
+    <t>Month-19</t>
+  </si>
+  <si>
+    <t>Month-20</t>
   </si>
 </sst>
 </file>
@@ -359,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -377,6 +401,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,11 +724,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +737,7 @@
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -766,13 +792,19 @@
       <c r="S1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -783,7 +815,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -794,30 +826,42 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
       <c r="H5">
+        <v>37500</v>
+      </c>
+      <c r="I5">
+        <v>75000</v>
+      </c>
+      <c r="J5">
         <v>150000</v>
       </c>
-      <c r="I5">
-        <v>150000</v>
-      </c>
-      <c r="J5">
+      <c r="K5">
         <v>75000</v>
       </c>
+      <c r="L5">
+        <v>37500</v>
+      </c>
       <c r="Q5">
-        <v>100000</v>
+        <v>37500</v>
       </c>
       <c r="R5">
-        <v>100000</v>
+        <v>67500</v>
       </c>
       <c r="S5">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>90000</v>
+      </c>
+      <c r="T5">
+        <v>67500</v>
+      </c>
+      <c r="U5">
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -826,7 +870,7 @@
         <v>150000</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:S7" si="0">SUM(C3:C5)</f>
+        <f t="shared" ref="C7:U7" si="0">SUM(C3:C5)</f>
         <v>0</v>
       </c>
       <c r="D7">
@@ -847,23 +891,23 @@
       </c>
       <c r="H7">
         <f>SUM(H3:H5)</f>
-        <v>150000</v>
+        <v>37500</v>
       </c>
       <c r="I7">
         <f>SUM(I3:I5)</f>
-        <v>150000</v>
+        <v>75000</v>
       </c>
       <c r="J7">
         <f>SUM(J3:J5)</f>
-        <v>75000</v>
+        <v>150000</v>
       </c>
       <c r="K7">
         <f>SUM(K3:K5)</f>
-        <v>50000</v>
+        <v>125000</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37500</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
@@ -883,23 +927,31 @@
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>37500</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>67500</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>90000</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>67500</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -949,7 +1001,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>38</v>
       </c>
@@ -972,7 +1024,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1022,7 +1074,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1072,7 +1124,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1122,7 +1174,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1145,7 +1197,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1161,14 +1213,8 @@
       <c r="E16">
         <v>2000</v>
       </c>
-      <c r="F16">
-        <v>2000</v>
-      </c>
-      <c r="G16">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1178,20 +1224,8 @@
       <c r="C17">
         <v>2000</v>
       </c>
-      <c r="D17">
-        <v>2000</v>
-      </c>
-      <c r="E17">
-        <v>2000</v>
-      </c>
-      <c r="F17">
-        <v>2000</v>
-      </c>
-      <c r="G17">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1210,23 +1244,20 @@
       <c r="F18">
         <v>2000</v>
       </c>
-      <c r="G18">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>10000</v>
-      </c>
-      <c r="G20">
-        <v>20000</v>
       </c>
       <c r="H20">
         <v>20000</v>
       </c>
+      <c r="I20">
+        <v>20000</v>
+      </c>
       <c r="P20">
         <v>50000</v>
       </c>
@@ -1237,35 +1268,53 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="H21">
-        <v>150000</v>
+        <v>37500</v>
+      </c>
+      <c r="I21">
+        <v>75000</v>
+      </c>
+      <c r="J21">
+        <v>37500</v>
       </c>
       <c r="Q21">
-        <v>100000</v>
+        <v>37500</v>
       </c>
       <c r="R21">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <v>67500</v>
+      </c>
+      <c r="S21">
+        <v>90000</v>
+      </c>
+      <c r="T21">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="I22">
-        <v>75000</v>
-      </c>
       <c r="J22">
+        <v>56250</v>
+      </c>
+      <c r="K22">
         <v>37500</v>
       </c>
-      <c r="S22">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>18750</v>
+      </c>
+      <c r="T22">
+        <v>31250</v>
+      </c>
+      <c r="U22">
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1279,46 +1328,46 @@
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>15200</v>
+        <v>13200</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>15200</v>
+        <v>13200</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>25200</v>
+        <v>11200</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>35200</v>
+        <v>19200</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
-        <v>177200</v>
+        <v>64700</v>
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
-        <v>82200</v>
+        <v>102200</v>
       </c>
       <c r="J24">
         <f t="shared" si="1"/>
-        <v>44700</v>
+        <v>100950</v>
       </c>
       <c r="K24">
         <f t="shared" si="1"/>
-        <v>7200</v>
+        <v>44700</v>
       </c>
       <c r="L24">
         <f t="shared" si="1"/>
-        <v>7200</v>
+        <v>25950</v>
       </c>
       <c r="M24">
         <f t="shared" si="1"/>
         <v>7200</v>
       </c>
       <c r="N24">
-        <f t="shared" ref="N24:S24" si="2">SUM(N10:N22)</f>
+        <f t="shared" ref="N24:U24" si="2">SUM(N10:N22)</f>
         <v>7200</v>
       </c>
       <c r="O24">
@@ -1331,18 +1380,26 @@
       </c>
       <c r="Q24">
         <f t="shared" si="2"/>
-        <v>150000</v>
+        <v>87500</v>
       </c>
       <c r="R24">
         <f t="shared" si="2"/>
-        <v>150000</v>
+        <v>117500</v>
       </c>
       <c r="S24">
         <f t="shared" si="2"/>
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+        <v>90000</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="2"/>
+        <v>36250</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="2"/>
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1356,19 +1413,19 @@
       </c>
       <c r="D26">
         <f t="shared" si="3"/>
-        <v>-15200</v>
+        <v>-13200</v>
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>-15200</v>
+        <v>-13200</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>-25200</v>
+        <v>-11200</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>-35200</v>
+        <v>-19200</v>
       </c>
       <c r="H26">
         <f t="shared" si="3"/>
@@ -1376,26 +1433,26 @@
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>67800</v>
+        <v>-27200</v>
       </c>
       <c r="J26">
         <f t="shared" si="3"/>
-        <v>30300</v>
+        <v>49050</v>
       </c>
       <c r="K26">
         <f t="shared" si="3"/>
-        <v>42800</v>
+        <v>80300</v>
       </c>
       <c r="L26">
         <f t="shared" si="3"/>
-        <v>-7200</v>
+        <v>11550</v>
       </c>
       <c r="M26">
         <f t="shared" si="3"/>
         <v>-7200</v>
       </c>
       <c r="N26">
-        <f t="shared" ref="N26:S26" si="4">N7-N24</f>
+        <f t="shared" ref="N26:U26" si="4">N7-N24</f>
         <v>-7200</v>
       </c>
       <c r="O26">
@@ -1416,10 +1473,18 @@
       </c>
       <c r="S26">
         <f t="shared" si="4"/>
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="4"/>
+        <v>31250</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="4"/>
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1433,71 +1498,79 @@
       </c>
       <c r="D28">
         <f t="shared" ref="D28:S28" si="5">C28+D26</f>
-        <v>104400</v>
+        <v>106400</v>
       </c>
       <c r="E28">
         <f t="shared" si="5"/>
-        <v>89200</v>
+        <v>93200</v>
       </c>
       <c r="F28">
         <f t="shared" si="5"/>
-        <v>64000</v>
+        <v>82000</v>
       </c>
       <c r="G28">
         <f t="shared" si="5"/>
-        <v>28800</v>
+        <v>62800</v>
       </c>
       <c r="H28">
         <f t="shared" si="5"/>
-        <v>1600</v>
+        <v>35600</v>
       </c>
       <c r="I28">
         <f t="shared" si="5"/>
-        <v>69400</v>
+        <v>8400</v>
       </c>
       <c r="J28">
         <f t="shared" si="5"/>
-        <v>99700</v>
+        <v>57450</v>
       </c>
       <c r="K28">
         <f t="shared" si="5"/>
-        <v>142500</v>
+        <v>137750</v>
       </c>
       <c r="L28">
         <f t="shared" si="5"/>
-        <v>135300</v>
+        <v>149300</v>
       </c>
       <c r="M28">
         <f t="shared" si="5"/>
-        <v>128100</v>
+        <v>142100</v>
       </c>
       <c r="N28">
         <f t="shared" si="5"/>
-        <v>120900</v>
+        <v>134900</v>
       </c>
       <c r="O28">
         <f t="shared" si="5"/>
-        <v>113700</v>
+        <v>127700</v>
       </c>
       <c r="P28">
         <f t="shared" si="5"/>
-        <v>206500</v>
+        <v>220500</v>
       </c>
       <c r="Q28">
         <f t="shared" si="5"/>
-        <v>156500</v>
+        <v>170500</v>
       </c>
       <c r="R28">
         <f t="shared" si="5"/>
-        <v>106500</v>
+        <v>120500</v>
       </c>
       <c r="S28">
         <f t="shared" si="5"/>
-        <v>156500</v>
+        <v>120500</v>
+      </c>
+      <c r="T28">
+        <f t="shared" ref="T28" si="6">S28+T26</f>
+        <v>151750</v>
+      </c>
+      <c r="U28">
+        <f t="shared" ref="U28" si="7">T28+U26</f>
+        <v>170500</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B26:S26">
+  <conditionalFormatting sqref="B26:U26">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1516,7 +1589,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K17" sqref="K17"/>
+      <selection pane="topRight" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,6 +1626,12 @@
       <c r="J1" t="s">
         <v>11</v>
       </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1580,13 +1659,19 @@
         <v>41</v>
       </c>
       <c r="H5">
-        <v>75000</v>
+        <v>22500</v>
       </c>
       <c r="I5">
-        <v>75000</v>
+        <v>52500</v>
       </c>
       <c r="J5">
         <v>75000</v>
+      </c>
+      <c r="K5">
+        <v>52500</v>
+      </c>
+      <c r="L5">
+        <v>22500</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1619,15 +1704,23 @@
       </c>
       <c r="H7">
         <f>SUM(H3:H5)</f>
-        <v>75000</v>
+        <v>22500</v>
       </c>
       <c r="I7">
         <f>SUM(I3:I5)</f>
-        <v>75000</v>
+        <v>52500</v>
       </c>
       <c r="J7">
         <f>SUM(J3:J5)</f>
         <v>75000</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:L7" si="1">SUM(K3:K5)</f>
+        <v>52500</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>22500</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1823,14 +1916,8 @@
       <c r="E16">
         <v>2000</v>
       </c>
-      <c r="F16">
-        <v>2000</v>
-      </c>
-      <c r="G16">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1840,14 +1927,8 @@
       <c r="C17">
         <v>2000</v>
       </c>
-      <c r="D17">
-        <v>2000</v>
-      </c>
-      <c r="E17">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1867,7 +1948,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1881,108 +1962,130 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="H21">
+        <v>22500</v>
+      </c>
+      <c r="I21">
+        <v>52500</v>
+      </c>
+      <c r="J21">
         <v>75000</v>
       </c>
-      <c r="I21">
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="J22">
-        <v>37500</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>26250</v>
+      </c>
+      <c r="L22">
+        <v>11250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B24">
-        <f t="shared" ref="B24:J24" si="1">SUM(B10:B22)</f>
+        <f t="shared" ref="B24:L24" si="2">SUM(B10:B22)</f>
         <v>15200</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15200</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
-        <v>15200</v>
+        <f t="shared" si="2"/>
+        <v>13200</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
-        <v>15200</v>
+        <f t="shared" si="2"/>
+        <v>13200</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
-        <v>23200</v>
+        <f t="shared" si="2"/>
+        <v>21200</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
-        <v>31200</v>
+        <f t="shared" si="2"/>
+        <v>29200</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
-        <v>102200</v>
+        <f t="shared" si="2"/>
+        <v>49700</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>59700</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
         <v>82200</v>
       </c>
-      <c r="J24">
-        <f t="shared" si="1"/>
-        <v>44700</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <f t="shared" si="2"/>
+        <v>26250</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>11250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:J26" si="2">B7-B24</f>
+        <f t="shared" ref="B26:L26" si="3">B7-B24</f>
         <v>134800</v>
       </c>
       <c r="C26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-15200</v>
       </c>
       <c r="D26">
-        <f t="shared" si="2"/>
-        <v>-15200</v>
+        <f t="shared" si="3"/>
+        <v>-13200</v>
       </c>
       <c r="E26">
-        <f t="shared" si="2"/>
-        <v>-15200</v>
+        <f t="shared" si="3"/>
+        <v>-13200</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
-        <v>-23200</v>
+        <f t="shared" si="3"/>
+        <v>-21200</v>
       </c>
       <c r="G26">
-        <f t="shared" si="2"/>
-        <v>-31200</v>
+        <f t="shared" si="3"/>
+        <v>-29200</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-27200</v>
       </c>
       <c r="I26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-7200</v>
       </c>
       <c r="J26">
-        <f t="shared" si="2"/>
-        <v>30300</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-7200</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="3"/>
+        <v>26250</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="3"/>
+        <v>11250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1995,36 +2098,44 @@
         <v>119600</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:J28" si="3">C28+D26</f>
-        <v>104400</v>
+        <f t="shared" ref="D28:J28" si="4">C28+D26</f>
+        <v>106400</v>
       </c>
       <c r="E28">
-        <f t="shared" si="3"/>
-        <v>89200</v>
+        <f t="shared" si="4"/>
+        <v>93200</v>
       </c>
       <c r="F28">
-        <f t="shared" si="3"/>
-        <v>66000</v>
+        <f t="shared" si="4"/>
+        <v>72000</v>
       </c>
       <c r="G28">
-        <f t="shared" si="3"/>
-        <v>34800</v>
+        <f t="shared" si="4"/>
+        <v>42800</v>
       </c>
       <c r="H28">
-        <f t="shared" si="3"/>
-        <v>7600</v>
+        <f t="shared" si="4"/>
+        <v>15600</v>
       </c>
       <c r="I28">
-        <f t="shared" si="3"/>
-        <v>400</v>
+        <f t="shared" si="4"/>
+        <v>8400</v>
       </c>
       <c r="J28">
-        <f t="shared" si="3"/>
-        <v>30700</v>
+        <f t="shared" si="4"/>
+        <v>1200</v>
+      </c>
+      <c r="K28">
+        <f t="shared" ref="K28" si="5">J28+K26</f>
+        <v>27450</v>
+      </c>
+      <c r="L28">
+        <f t="shared" ref="L28" si="6">K28+L26</f>
+        <v>38700</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B26:J26">
+  <conditionalFormatting sqref="B26:L26">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2662,7 +2773,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2898,13 +3009,866 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>3000</v>
+      </c>
+      <c r="C4">
+        <v>7000</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+      <c r="E4">
+        <v>7000</v>
+      </c>
+      <c r="F4">
+        <v>3000</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4">
+        <v>5000</v>
+      </c>
+      <c r="J4">
+        <v>10000</v>
+      </c>
+      <c r="K4">
+        <v>20000</v>
+      </c>
+      <c r="L4">
+        <v>10000</v>
+      </c>
+      <c r="M4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>7.5</v>
+      </c>
+      <c r="C5">
+        <v>7.5</v>
+      </c>
+      <c r="D5">
+        <v>7.5</v>
+      </c>
+      <c r="E5">
+        <v>7.5</v>
+      </c>
+      <c r="F5">
+        <v>7.5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5">
+        <v>7.5</v>
+      </c>
+      <c r="J5">
+        <v>7.5</v>
+      </c>
+      <c r="K5">
+        <v>7.5</v>
+      </c>
+      <c r="L5">
+        <v>7.5</v>
+      </c>
+      <c r="M5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="4">
+        <f>B5*B4</f>
+        <v>22500</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" ref="C6:F6" si="0">C5*C4</f>
+        <v>52500</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>75000</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>52500</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>22500</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="4">
+        <f>I5*I4</f>
+        <v>37500</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" ref="J6:M6" si="1">J5*J4</f>
+        <v>75000</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" si="1"/>
+        <v>150000</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="1"/>
+        <v>75000</v>
+      </c>
+      <c r="M6" s="4">
+        <f t="shared" si="1"/>
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="7">
+        <f>B6</f>
+        <v>22500</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" ref="C8:F8" si="2">C6</f>
+        <v>52500</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="2"/>
+        <v>75000</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="2"/>
+        <v>52500</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="2"/>
+        <v>22500</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="7">
+        <f>I6</f>
+        <v>37500</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" ref="J8:M8" si="3">J6</f>
+        <v>75000</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="3"/>
+        <v>150000</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="3"/>
+        <v>75000</v>
+      </c>
+      <c r="M8" s="7">
+        <f t="shared" si="3"/>
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11">
+        <v>22500</v>
+      </c>
+      <c r="C11">
+        <v>52500</v>
+      </c>
+      <c r="D11">
+        <v>75000</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11">
+        <v>37500</v>
+      </c>
+      <c r="J11">
+        <v>75000</v>
+      </c>
+      <c r="K11">
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12">
+        <f>(B8-B11)*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:F12" si="4">(C8-C11)*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
+        <v>26250</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>11250</v>
+      </c>
+      <c r="H12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12">
+        <f>(I8-I11)*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ref="J12" si="5">(J8-J11)*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ref="K12" si="6">(K8-K11)*0.5</f>
+        <v>56250</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ref="L12" si="7">(L8-L11)*0.5</f>
+        <v>37500</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ref="M12" si="8">(M8-M11)*0.5</f>
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="7">
+        <f>B11+B12</f>
+        <v>22500</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" ref="C14:F14" si="9">C11+C12</f>
+        <v>52500</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="9"/>
+        <v>75000</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="9"/>
+        <v>26250</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="9"/>
+        <v>11250</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="7">
+        <f>I11+I12</f>
+        <v>37500</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" ref="J14:M14" si="10">J11+J12</f>
+        <v>75000</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="10"/>
+        <v>93750</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="10"/>
+        <v>37500</v>
+      </c>
+      <c r="M14" s="7">
+        <f t="shared" si="10"/>
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16">
+        <f>B8-B14</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:F16" si="11">C8-C14</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="11"/>
+        <v>26250</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="11"/>
+        <v>11250</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16">
+        <f>I8-I14</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16:M16" si="12">J8-J14</f>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="12"/>
+        <v>56250</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="12"/>
+        <v>37500</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="12"/>
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="7">
+        <f>B16</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="7">
+        <f>C16+B18</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" ref="D18:F18" si="13">D16+C18</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="13"/>
+        <v>26250</v>
+      </c>
+      <c r="F18" s="7">
+        <f t="shared" si="13"/>
+        <v>37500</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="7">
+        <f>I16</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="7">
+        <f>J16+I18</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" ref="K18" si="14">K16+J18</f>
+        <v>56250</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" ref="L18" si="15">L16+K18</f>
+        <v>93750</v>
+      </c>
+      <c r="M18" s="7">
+        <f t="shared" ref="M18" si="16">M16+L18</f>
+        <v>112500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <f>SUM(I11:M11)</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <v>2500</v>
+      </c>
+      <c r="C25">
+        <v>4500</v>
+      </c>
+      <c r="D25">
+        <v>6000</v>
+      </c>
+      <c r="E25">
+        <v>4500</v>
+      </c>
+      <c r="F25">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="4">
+        <f>B26*B25</f>
+        <v>12500</v>
+      </c>
+      <c r="C27" s="4">
+        <f>C26*C25</f>
+        <v>22500</v>
+      </c>
+      <c r="D27" s="4">
+        <f>D26*D25</f>
+        <v>30000</v>
+      </c>
+      <c r="E27" s="4">
+        <f>E26*E25</f>
+        <v>22500</v>
+      </c>
+      <c r="F27" s="4">
+        <f>F26*F25</f>
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30">
+        <v>2500</v>
+      </c>
+      <c r="C30">
+        <v>4500</v>
+      </c>
+      <c r="D30">
+        <v>6000</v>
+      </c>
+      <c r="E30">
+        <v>4500</v>
+      </c>
+      <c r="F30">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="4">
+        <f>B31*B30</f>
+        <v>12500</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" ref="C32:F32" si="17">C31*C30</f>
+        <v>22500</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="17"/>
+        <v>30000</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" si="17"/>
+        <v>22500</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" si="17"/>
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35">
+        <v>2500</v>
+      </c>
+      <c r="C35">
+        <v>4500</v>
+      </c>
+      <c r="D35">
+        <v>6000</v>
+      </c>
+      <c r="E35">
+        <v>4500</v>
+      </c>
+      <c r="F35">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="4">
+        <f>B36*B35</f>
+        <v>12500</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" ref="C37:F37" si="18">C36*C35</f>
+        <v>22500</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="18"/>
+        <v>30000</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="18"/>
+        <v>22500</v>
+      </c>
+      <c r="F37" s="4">
+        <f t="shared" si="18"/>
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="7">
+        <f>B27+B32+B37</f>
+        <v>37500</v>
+      </c>
+      <c r="C39" s="7">
+        <f t="shared" ref="C39:F39" si="19">C27+C32+C37</f>
+        <v>67500</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" si="19"/>
+        <v>90000</v>
+      </c>
+      <c r="E39" s="7">
+        <f t="shared" si="19"/>
+        <v>67500</v>
+      </c>
+      <c r="F39" s="7">
+        <f t="shared" si="19"/>
+        <v>37500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42">
+        <v>37500</v>
+      </c>
+      <c r="C42">
+        <v>67500</v>
+      </c>
+      <c r="D42">
+        <v>90000</v>
+      </c>
+      <c r="E42">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43">
+        <f>(B39-B42)*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ref="C43:F43" si="20">(C39-C42)*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="20"/>
+        <v>31250</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="20"/>
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="7">
+        <f>B42+B43</f>
+        <v>37500</v>
+      </c>
+      <c r="C45" s="7">
+        <f t="shared" ref="C45:F45" si="21">C42+C43</f>
+        <v>67500</v>
+      </c>
+      <c r="D45" s="7">
+        <f t="shared" si="21"/>
+        <v>90000</v>
+      </c>
+      <c r="E45" s="7">
+        <f t="shared" si="21"/>
+        <v>36250</v>
+      </c>
+      <c r="F45" s="7">
+        <f t="shared" si="21"/>
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47">
+        <f>B39-B45</f>
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ref="C47:F47" si="22">C39-C45</f>
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="22"/>
+        <v>31250</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="22"/>
+        <v>18750</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="7">
+        <f>B47</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="7">
+        <f>C47+B49</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" ref="D49" si="23">D47+C49</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="7">
+        <f t="shared" ref="E49" si="24">E47+D49</f>
+        <v>31250</v>
+      </c>
+      <c r="F49" s="7">
+        <f t="shared" ref="F49" si="25">F47+E49</f>
+        <v>50000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2912,7 +3876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>